<commit_message>
updated files in git
</commit_message>
<xml_diff>
--- a/web/CHD_Guidelines_and_Release_Notes.xlsx
+++ b/web/CHD_Guidelines_and_Release_Notes.xlsx
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,26 +73,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Scroll right side to see various cases.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>Greenhouse Gas Management Institute Revisualization and localization US21838 44493_alpha_03_11_2016_T08_01_30.jpg</t>
   </si>
@@ -894,15 +880,6 @@
   </si>
   <si>
     <t xml:space="preserve">Partial Testing </t>
-  </si>
-  <si>
-    <t>Onscreen Text Mapping/Functionality/Audio Review/Audio Mapping/Audio Syncing/Transcript Mapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regression Testing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCORM Testing </t>
   </si>
   <si>
     <r>
@@ -1028,9 +1005,6 @@
     <t>Provide all developer names from each function who are involved in the development of respective course.</t>
   </si>
   <si>
-    <t>Total number of screen count/40</t>
-  </si>
-  <si>
     <t>Provide correct and complete SVN path of the course to be tested.</t>
   </si>
   <si>
@@ -1038,729 +1012,6 @@
   </si>
   <si>
     <t>Provide any supporting document here. Better to place all supporting documents on SVN and share the path in CHD.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Proto: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Choose this when a prototype id being submitted to customer.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">POC: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Proof of concept-&gt;Use this phase when we are  submitting a course with few pages for bidding a deal.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alpha:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Use this phase when there is 1st time submission to customer.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Beta: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Use this phase when there is 2nd and beyond submission to customer.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Gold: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Use this phase when there is final submission to customer including SCORM version of the course.</t>
-    </r>
-  </si>
-  <si>
-    <t>Specify complete set of OS-Browser combinations where testing is to be performed as per customer requirement.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For 1st time feedback from customer choose Clientedit Alpha. For all subsequent submissions to customer, choose Clientedit Beta. For final/last set of changes choose Clientedit Gold.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">For example: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Case 1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-First time submission to customer and QC then,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Alpha
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Scope of Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= E2E
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Partial Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= Onscreen Text Mapping, Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Regression Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Do not select any option here.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Case 3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-First time feedback from customer with huge list of changes and complete revision of course content is received. Audio is not yet recorded and added to course because of huge number of changes. All client edit fixes verification along with complete mapping is expected in this round.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Beta
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Scope of Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= Partial Testing
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Partial Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Onscreen Text Mapping, Functionality, Transcript Mapping
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Regression Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Clientedit Alpha</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Case 4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Second time feedback from customer with quite a few number of changes received. Audio is not yet recorded. All client edit fixes verification along with complete mapping is expected in this round.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Beta
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Scope of Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= Regression Testing
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Partial Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Functionality
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Regression Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Clientedit Beta</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Case 5:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Second (and beyond) time feedback from customer with few number of changes received. Audio is recorded. All client edit fixes verification along with audio testing is expected in this round.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Beta
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Scope of Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= Partial Testing
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Partial Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Regression Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Clientedit Beta</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Case 5:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Final feedback from customer with few number of changes received. SCORM is implemented. All client edit fixes verification along with SCORM testing is expected in this round.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Gold
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Scope of Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= Partial Testing
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Partial Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Regression Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Clientedit Beta
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">SCORM Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= Scorm #/AICC testing (Mention as applicable.</t>
-    </r>
   </si>
   <si>
     <t>1. Global Guidelines: Please avoid special characters in the project name, course name, release notes or any part of the CHD.
@@ -1769,143 +1020,6 @@
   </si>
   <si>
     <t>Provide correct and complete SVN path of the latest storyboard to be referred to including the respective file name. Provide correct and complete SVN path of the base course provided by customer to be referred to as applicable.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Case 2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-First time feedback from customer where there are less number of changes received, so along with implementing changes we have also added audio to the course  then,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Beta
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Scope of Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= Partial Testing
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Partial Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Regression Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Clientedit Alpha
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Release Notes:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Please mention all exceptions clearly here. </t>
-    </r>
-  </si>
-  <si>
-    <t>Select Scorm 1.2, Scorm 2004, AICC as applicable.</t>
   </si>
   <si>
     <t xml:space="preserve">Choose correct course level as applicable for respective course. </t>
@@ -2192,15 +1306,505 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Case 5:</t>
+      <t xml:space="preserve">No of Slides/Pages in Storyboard </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Provide correct number of SB slides/pages here.</t>
+  </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Map viz notes in SB.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTE: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>By default, QC does not map the viz notes. Their focus is to test the sceen from user perspective. Viz notes section should be closed within devlopment teams.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Generic Test cases SVN path: http://192.168.2.4/content3/QC/Checklist/Updated Checklist/QC Generic Test Cases_V2.xlsx
+&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provide project specific customized test cases path that you have used for self review. In absence of customized checklist, you can use applicable checkpoints from generic test cases.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>For Scorm testing, use Wisdom LMS because client use the same.</t>
+  </si>
+  <si>
+    <t>Branching: On the click of Prev/Back button, screen will jump to the Last Visited page instead of immediate previous page.</t>
+  </si>
+  <si>
+    <t>Provide correct Project name along with PIN details. If you do not see the project listed, please connect with SEPG team to get the respective project assigned to you.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Technology limitation (Storyline/lectora/flash/HTML5 limitation)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;Dev team to specify any tool limitation here. To start with QC team has collated some S/W constraints in the xls below, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>however, this list is not yet formally approved by media team.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Please specify any additional constraints that is not part of this list and applicable to the course. Please note that some of the issues in this list are not S/W constraint, however, if dev manager has decided not to fix them due to time constraint then mention the relevant reason for keeping such issues as open upfront.&gt; In absence of release notes, QC will raise them as issues.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide correct size of course folder here excluding the source size.
+</t>
+  </si>
+  <si>
+    <t>Developer Names[ID]</t>
+  </si>
+  <si>
+    <t>Developer Names[Med]</t>
+  </si>
+  <si>
+    <t>Choose all ID names who have worked on this project and are accountable for quality of the course.</t>
+  </si>
+  <si>
+    <t>Choose all media developer names who have worked on this project and are accountable for quality of the course.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Proto: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Choose this when a prototype id being submitted to customer. When you choose this phase the client edits option will remain disabled.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">POC: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Proof of concept-&gt;Use this phase when we are  submitting a course with few pages for bidding a deal. When you choose this phase the client edits option will remain disabled.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alpha:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Use this phase when there is 1st time submission to customer. When you choose this phase the client edits option will remain disabled.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Beta: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Use this phase when there is 2nd and beyond submission to customer. The client edits option will be enabled for this phase.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Gold: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Use this phase when there is final submission to customer including SCORM version of the course. The client edits option will be enabled for this phase.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We have some instances where screen count of constructed course is much less than the number of slides in SB. 
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Case to be considered: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Single screen with layered content; simulations; videos; animations; popup heavy screens with each popup containing content equivalent to one page/frame/screen.
+To calculate frame count of such courses please use the following method:
+Total Frame Count = Frame count in the SB + (Audio word count of the animation/Words count per page depending on the level of course). 
+The standard word count is L1 – 125, L2 – 135, and L3 – 150.
+2. For videos, LH will the the video duration/60; use following calculation for screen count:
+(Video duration/60)*40
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Total number of HTML or Flash Pages/40</t>
+  </si>
+  <si>
+    <t>Content mapping/Functionality/Audio review/Audio mapping/Audio syncing/Transcript mapping/Scorm 1.2/Scorm 2004/AICC/ILT/Internal edit/Clientedit alpha/Clientedit beta/Clientedit gold/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+First time feedback from customer where there are less number of changes received, so along with implementing changes we have also added audio to the course  then,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Beta
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scope of Testing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= Partial Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partial Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Clientedit Alpha
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Release Notes:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Please mention all exceptions clearly here. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Choose relevant scope applicable for respective module. For 1st time feedback from customer choose Clientedit Alpha. For all subsequent submissions to customer, choose Clientedit Beta. For final/last set of changes choose Clientedit Gold.
+Case 1: 
+First time submission to customer and QC then,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Alpha
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Scope of Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = E2E
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Partial Testing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= Onscreen Text Mapping, Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 7:</t>
     </r>
     <r>
       <rPr>
@@ -2277,151 +1881,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = Functionality
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Regression Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Do not select any option here.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">SCORM Testing </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= Scorm #/AICC testing (Mention as applicable.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">No of Slides/Pages in Storyboard </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Provide correct number of SB slides/pages here.</t>
-  </si>
-  <si>
-    <t>Programmer</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Map viz notes in SB.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">NOTE: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>By default, QC does not map the viz notes. Their focus is to test the sceen from user perspective. Viz notes section should be closed within devlopment teams.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Generic Test cases SVN path: http://192.168.2.4/content3/QC/Checklist/Updated Checklist/QC Generic Test Cases_V2.xlsx
-&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provide project specific customized test cases path that you have used for self review. In absence of customized checklist, you can use applicable checkpoints from generic test cases.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>For Scorm testing, use Wisdom LMS because client use the same.</t>
-  </si>
-  <si>
-    <t>Branching: On the click of Prev/Back button, screen will jump to the Last Visited page instead of immediate previous page.</t>
-  </si>
-  <si>
-    <t>Provide correct Project name along with PIN details. If you do not see the project listed, please connect with SEPG team to get the respective project assigned to you.</t>
-  </si>
-  <si>
-    <t>Provide correct size of course folder here excluding the source size.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Technology limitation (Storyline/lectora/flash/HTML5 limitation)</t>
+      <t xml:space="preserve"> = Functionality, Scorm #/AICC testing (Select as applicable.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 6:</t>
     </r>
     <r>
       <rPr>
@@ -2432,29 +1905,360 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-&lt;Dev team to specify any tool limitation here. To start with QC team has collated some S/W constraints in the xls below, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>however, this list is not yet formally approved by media team.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Please specify any additional constraints that is not part of this list and applicable to the course. Please note that some of the issues in this list are not S/W constraint, however, if dev manager has decided not to fix them due to time constraint then mention the relevant reason for keeping such issues as open upfront.&gt; In absence of release notes, QC will raise them as issues.</t>
-    </r>
+Final feedback from customer with few number of changes received. SCORM is implemented. All client edit fixes verification along with SCORM testing is expected in this round.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Gold
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scope of Testing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= Partial Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partial Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping, Clientedit Beta, Scorm #/AICC testing (Select as applicable.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 5:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Second (and beyond) time feedback from customer with few number of changes received. Audio is recorded. All client edit fixes verification along with audio testing is expected in this round.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Beta
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scope of Testing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= Partial Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partial Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Functionality, Audio Review, Audio Mapping, Audio Syncing, Transcript Mapping,  Clientedit Beta</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Second time feedback from customer with quite a few number of changes received. Audio is not yet recorded. All client edit fixes verification along with complete mapping is expected in this round.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Beta
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scope of Testing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= Regression Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partial Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Functionality, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clientedit Beta</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+First time feedback from customer with huge list of changes and complete revision of course content is received. Audio is not yet recorded and added to course because of huge number of changes. All client edit fixes verification along with complete mapping is expected in this round.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Beta
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scope of Testing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= Partial Testing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partial Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Onscreen Text Mapping, Functionality, Transcript Mapping, Clientedit Alpha</t>
+    </r>
+  </si>
+  <si>
+    <t>Components should be signedoff by respective functions post selv review and before it is submitted to QC. Choose relevant option here. Peer review without functioonal signoff, if selected, should have exception from DM and SPM.</t>
+  </si>
+  <si>
+    <t>Specify complete set of OS-Browser combinations where testing is to be performed as per customer requirement. Select all applicbale environment here. In case one off the selected devices is applicable, please mention this information in release notes clearly to QC.</t>
   </si>
 </sst>
 </file>
@@ -3206,7 +3010,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3214,7 +3018,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -3222,7 +3026,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3230,7 +3034,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -3238,7 +3042,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3246,7 +3050,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
@@ -3256,7 +3060,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3264,7 +3068,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3272,7 +3076,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D11" s="13"/>
     </row>
@@ -3281,7 +3085,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -3291,7 +3095,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -3301,7 +3105,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3309,7 +3113,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
@@ -3319,7 +3123,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -3327,7 +3131,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
@@ -3337,10 +3141,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D18" s="19"/>
     </row>
@@ -3349,7 +3153,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
@@ -3359,7 +3163,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -3367,7 +3171,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -3375,7 +3179,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -3383,10 +3187,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -3394,7 +3198,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -3402,7 +3206,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3448,13 +3252,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3464,7 +3268,7 @@
     <col min="3" max="6" width="78.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="48.5703125" style="4" customWidth="1"/>
     <col min="8" max="8" width="53.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3474,7 +3278,7 @@
     </row>
     <row r="2" spans="1:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B2" s="26"/>
     </row>
@@ -3488,7 +3292,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3496,7 +3300,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3504,7 +3308,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
@@ -3512,7 +3316,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3520,7 +3324,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3528,238 +3332,270 @@
         <v>29</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+    <row r="16" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="C16" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="B17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B22" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="B23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>59</v>
+      <c r="C23" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>50</v>
-      </c>
       <c r="B30" s="13" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+        <v>46</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
       <formula1>"E2E, Regression Testing, Partial Testing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
       <formula1>"L1, L2, L3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
-      <formula1>"SCORM 1.2, SCORM 2004, AICC Testing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
-      <formula1>"Clientedit Alpha, Clientedit Beta, Clientedit Gold"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
       <formula1>"Proto, POC, Alpha, Beta, Gold"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B29" location="'Release Notes'!A1" display="Refer to the Release Notes tab for samples and add all applicable release notes for respective course  here."/>
+    <hyperlink ref="B31" location="'Release Notes'!A1" display="Refer to the Release Notes tab for samples and add all applicable release notes for respective course  here."/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>